<commit_message>
Complete white-box testing documentation for Lab03
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E816B38A-AEDB-4F02-8E52-FF85D165F6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F7AEBC-8C24-4F1E-9533-F13B53DBAB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="141">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -183,15 +183,6 @@
     <t>Loop (lc)</t>
   </si>
   <si>
-    <t>F02_Cond01 &gt; 100</t>
-  </si>
-  <si>
-    <t>F02_Cond02 &lt; 20</t>
-  </si>
-  <si>
-    <t>F02_Cond03 == i</t>
-  </si>
-  <si>
     <t>F02_Condnn &lt; n</t>
   </si>
   <si>
@@ -217,12 +208,6 @@
   </si>
   <si>
     <t>F02_TC01</t>
-  </si>
-  <si>
-    <t>1, 2,4, 6, 7</t>
-  </si>
-  <si>
-    <t>F01_TC02</t>
   </si>
   <si>
     <t>WBT Implemented TCs</t>
@@ -524,6 +509,145 @@
   </si>
   <si>
     <t>F02.  La inchiderea restaurantului se afiseaza totalul incasarilor realizate, pentru fiecare tip de plata.</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Cash</t>
+  </si>
+  <si>
+    <t>Sum of all Cash payments</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6, 8, 9, 10, 11</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>F02_TC03</t>
+  </si>
+  <si>
+    <t>F02_TC04</t>
+  </si>
+  <si>
+    <t>F02_TC05</t>
+  </si>
+  <si>
+    <t>F02_TC06</t>
+  </si>
+  <si>
+    <t>F02_TC07</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Card</t>
+  </si>
+  <si>
+    <t>type = null</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Cash, payments = empty list</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Cash, payments contains both Cash and Card payments</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Cash, payments contains only Card payments</t>
+  </si>
+  <si>
+    <t>type = PaymentType.Cash, payments = null</t>
+  </si>
+  <si>
+    <t>Sum of all Card payments</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Sum of Cash payments only</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6, 8, 9, 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F02_Cond01: type invalid
+</t>
+  </si>
+  <si>
+    <t>F02_Cond02: payments empty</t>
+  </si>
+  <si>
+    <t>F02_Cond03: payment type matches</t>
+  </si>
+  <si>
+    <t>F02_TC08</t>
+  </si>
+  <si>
+    <t>F02_TC09</t>
+  </si>
+  <si>
+    <t>F02_TC10</t>
+  </si>
+  <si>
+    <t>F02_TC11</t>
+  </si>
+  <si>
+    <t>F02_TC12</t>
+  </si>
+  <si>
+    <t>F02_TC13</t>
+  </si>
+  <si>
+    <t>tableNumber</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>PaymentType.Cash</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>25.5</t>
+  </si>
+  <si>
+    <t>22.3</t>
+  </si>
+  <si>
+    <t>PaymentType.Card</t>
+  </si>
+  <si>
+    <t>Non-empty menu list</t>
+  </si>
+  <si>
+    <t>Non-empty payment list</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException: "Invalid payment type"</t>
+  </si>
+  <si>
+    <t>Payment successfully added</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException: "Table number"</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException: "Payment type"</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException: "amount"</t>
   </si>
 </sst>
 </file>
@@ -666,7 +790,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,8 +863,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -749,32 +879,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -809,19 +913,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -932,19 +1023,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="double">
         <color indexed="64"/>
       </right>
@@ -1042,19 +1120,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -1100,145 +1165,54 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1247,184 +1221,182 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2208,7 +2180,7 @@
   </sheetPr>
   <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2218,16 +2190,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2235,31 +2207,31 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29" t="s">
+      <c r="N6" s="15"/>
+      <c r="O6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2268,13 +2240,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="P7" s="29">
+      <c r="O7" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="P7" s="15">
         <v>232</v>
       </c>
     </row>
@@ -2283,44 +2255,44 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="P8" s="29">
+      <c r="O8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="15">
         <v>232</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="P9" s="29">
+      <c r="O9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="15">
         <v>232</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="100" t="s">
-        <v>94</v>
+      <c r="B10" t="s">
+        <v>89</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="39" t="s">
-        <v>95</v>
+      <c r="B11" s="24" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2353,8 +2325,8 @@
   </sheetPr>
   <dimension ref="B1:Y41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="G26" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AF23" sqref="AF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2366,260 +2338,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="V6" s="42" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="V6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="L8" s="42" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="L8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="V8" s="50" t="s">
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="V8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="36">
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="V9" s="50" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="V9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="36" t="s">
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="L10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="V10" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="W10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="L11" s="25"/>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="V13" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="V15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="W15" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="V16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="W16" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+    </row>
+    <row r="17" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="W17" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+    </row>
+    <row r="18" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+    </row>
+    <row r="19" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V19" s="22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="49" t="s">
+      <c r="W19" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+    </row>
+    <row r="20" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V20" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="W20" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+    </row>
+    <row r="21" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V21" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="W21" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="L10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="W10" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="L11" s="40"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B13" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="V13" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B14" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="V15" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="W15" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="V16" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="W16" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-    </row>
-    <row r="17" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V17" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="W17" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-    </row>
-    <row r="18" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V18" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="W18" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="X18" s="45"/>
-      <c r="Y18" s="45"/>
-    </row>
-    <row r="19" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V19" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="W19" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="X19" s="45"/>
-      <c r="Y19" s="45"/>
-    </row>
-    <row r="20" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V20" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="W20" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
-    </row>
-    <row r="21" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V21" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="W21" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
     </row>
     <row r="41" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U41" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="W16:Y16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="W20:Y20"/>
     <mergeCell ref="W21:Y21"/>
@@ -2635,6 +2599,14 @@
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="W17:Y17"/>
     <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="W16:Y16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2649,8 +2621,8 @@
   </sheetPr>
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,433 +2649,560 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+    </row>
+    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+    </row>
+    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="79"/>
+      <c r="H8" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="38"/>
+      <c r="P8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="R8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="41">
+        <v>0</v>
+      </c>
+      <c r="W8" s="41">
+        <v>1</v>
+      </c>
+      <c r="X8" s="41">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z8" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA8" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB8" s="41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="X10" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y10" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z10" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA10" s="71"/>
+      <c r="AB10" s="71"/>
+    </row>
+    <row r="11" spans="2:28" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="X11" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y11" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z11" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="71"/>
+    </row>
+    <row r="12" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="52"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="W7" s="55"/>
-      <c r="X7" s="55"/>
-      <c r="Y7" s="55"/>
-      <c r="Z7" s="55"/>
-      <c r="AA7" s="55"/>
-      <c r="AB7" s="55"/>
-    </row>
-    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="52"/>
-      <c r="C8" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="60"/>
-      <c r="F8" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="59"/>
-      <c r="P8" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="V8" s="55">
-        <v>0</v>
-      </c>
-      <c r="W8" s="55">
-        <v>1</v>
-      </c>
-      <c r="X8" s="55">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z8" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA8" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB8" s="55" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="52"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="55"/>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="55"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-    </row>
-    <row r="11" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
-    </row>
-    <row r="12" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19"/>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="19"/>
-    </row>
-    <row r="13" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-    </row>
-    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
-    </row>
-    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
-    </row>
-    <row r="16" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
+      <c r="C12" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="71"/>
+      <c r="AB12" s="71"/>
+    </row>
+    <row r="13" spans="2:28" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="W13" s="71"/>
+      <c r="X13" s="71"/>
+      <c r="Y13" s="71"/>
+      <c r="Z13" s="71"/>
+      <c r="AA13" s="71"/>
+      <c r="AB13" s="71"/>
+    </row>
+    <row r="14" spans="2:28" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="X14" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y14" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z14" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA14" s="71"/>
+      <c r="AB14" s="71"/>
+    </row>
+    <row r="15" spans="2:28" ht="78" x14ac:dyDescent="0.3">
+      <c r="B15" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="X15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z15" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA15" s="71"/>
+      <c r="AB15" s="71"/>
+    </row>
+    <row r="16" spans="2:28" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="74"/>
+      <c r="G16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="S16" s="75"/>
+      <c r="T16" s="75"/>
+      <c r="U16" s="75"/>
+      <c r="V16" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="W16" s="76"/>
+      <c r="X16" s="76"/>
+      <c r="Y16" s="76"/>
+      <c r="Z16" s="76"/>
+      <c r="AA16" s="76"/>
+      <c r="AB16" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
+  <mergeCells count="31">
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -3120,6 +3219,20 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="V7:AB7"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="P7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3131,10 +3244,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3152,398 +3265,461 @@
     <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="63" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="64" t="s">
+      <c r="L4" s="47"/>
+    </row>
+    <row r="5" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="K5" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="L5" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="75" t="s">
+    </row>
+    <row r="6" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="27">
+        <v>1</v>
+      </c>
+      <c r="C6" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="D6" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="47"/>
+      <c r="K6" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="27">
+        <v>2</v>
+      </c>
+      <c r="C7" s="82"/>
+      <c r="D7" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="47"/>
+      <c r="K7" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="27">
+        <v>3</v>
+      </c>
+      <c r="C8" s="82"/>
+      <c r="D8" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="47"/>
+      <c r="K8" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B9" s="27">
+        <v>4</v>
+      </c>
+      <c r="C9" s="82"/>
+      <c r="D9" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="27">
+        <v>9</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="K9" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B10" s="27">
+        <v>5</v>
+      </c>
+      <c r="C10" s="82"/>
+      <c r="D10" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="27">
+        <v>8</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="27">
+        <v>6</v>
+      </c>
+      <c r="C11" s="82"/>
+      <c r="D11" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="27">
+        <v>8</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="27">
+        <v>-10</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="83">
+        <v>7</v>
+      </c>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="84" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="84"/>
+    </row>
+    <row r="13" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="83">
+        <v>8</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="66" t="s">
+      <c r="E13" s="84"/>
+      <c r="F13" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="84"/>
+    </row>
+    <row r="14" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="83">
+        <v>9</v>
+      </c>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="84"/>
+      <c r="F14" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="84"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="L14" s="84"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="67"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="69"/>
-      <c r="K5" s="2" t="s">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="52" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
+      <c r="G17" s="53"/>
+      <c r="H17" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="67"/>
+    </row>
+    <row r="18" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="N18" s="55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="45"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="50"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="15">
         <v>9</v>
       </c>
-      <c r="C6" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="78"/>
-      <c r="K6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="23">
-        <v>10</v>
-      </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="23">
-        <v>5</v>
-      </c>
-      <c r="F7" s="23">
-        <v>6</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="23">
-        <v>11</v>
-      </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="67"/>
-      <c r="K8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="23">
-        <v>12</v>
-      </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="2">
-        <v>13</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="69"/>
-      <c r="K10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="82"/>
-      <c r="H13" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="N13" s="62"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="87" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="93" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="84" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="85" t="s">
+      <c r="C20" s="13">
+        <v>9</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="85">
+        <v>1</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="87" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="89" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="97" t="s">
-        <v>80</v>
-      </c>
-      <c r="M14" s="99" t="s">
-        <v>81</v>
-      </c>
-      <c r="N14" s="73" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="92"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="84"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="29">
-        <f>SUM(C16:D16)</f>
+      <c r="H20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="15">
+        <f>SUM(J20:K20)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="26">
+      <c r="J20" s="13">
         <v>0</v>
       </c>
-      <c r="D16" s="26">
+      <c r="K20" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="29">
-        <f>SUM(J16:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="26">
-        <v>0</v>
-      </c>
-      <c r="K16" s="30">
-        <v>0</v>
-      </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N16" s="32">
-        <f>C16</f>
-        <v>0</v>
+      <c r="L20" s="86">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N20" s="17">
+        <f>C20</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
+  <mergeCells count="35">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:C10"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3551,7 +3727,22 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3559,21 +3750,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3717,24 +3893,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3750,4 +3924,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>